<commit_message>
go or stop function
</commit_message>
<xml_diff>
--- a/images/Book1.xlsx
+++ b/images/Book1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\my_develop2\python_basic\images\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C14B92F-907A-40A7-82DB-840BD9C6BEA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B28BD64A-262A-457A-A66C-2A2C79EC58AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{0499FA48-C906-448C-A146-6D45884876FE}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -49,6 +49,12 @@
       <family val="2"/>
       <charset val="129"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF000000"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="8"/>
@@ -112,18 +118,30 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp1.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp2.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp3.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp4.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp5.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp6.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp7.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
 </file>
 
@@ -147,7 +165,7 @@
         <xdr:cNvPr id="12" name="Picture 11">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1778230A-DC8E-46B8-BE69-50B3CAA96EB1}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000C000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -197,7 +215,7 @@
         <xdr:cNvPr id="16" name="Picture 15">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F6BA60E2-F94A-4EB6-834A-BA82B6AD4423}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000010000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -247,7 +265,7 @@
         <xdr:cNvPr id="17" name="Picture 16">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2D1A8257-8F35-4330-AEB0-22DADEC97DF0}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000011000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -297,7 +315,7 @@
         <xdr:cNvPr id="18" name="Picture 17">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{29A3455D-F2FD-4B5D-8EB4-A8CA668DFA2A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000012000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -334,101 +352,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>3</xdr:col>
-          <xdr:colOff>57148</xdr:colOff>
-          <xdr:row>14</xdr:row>
-          <xdr:rowOff>99806</xdr:rowOff>
+          <xdr:colOff>57150</xdr:colOff>
+          <xdr:row>15</xdr:row>
+          <xdr:rowOff>19050</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>525531</xdr:colOff>
-          <xdr:row>15</xdr:row>
-          <xdr:rowOff>107674</xdr:rowOff>
-        </xdr:to>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="1025" name="Check Box 1" hidden="1">
-              <a:extLst>
-                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s1025"/>
-                </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000001040000}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr/>
-          </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
-            <a:xfrm>
-              <a:off x="0" y="0"/>
-              <a:ext cx="0" cy="0"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
-          </xdr:spPr>
-          <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr algn="l" rtl="0">
-                <a:defRPr sz="1000"/>
-              </a:pPr>
-              <a:r>
-                <a:rPr lang="ko-KR" altLang="en-US" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
-                  <a:solidFill>
-                    <a:srgbClr val="000000"/>
-                  </a:solidFill>
-                  <a:latin typeface="Segoe UI"/>
-                  <a:cs typeface="Segoe UI"/>
-                </a:rPr>
-                <a:t>Check Box 1</a:t>
-              </a:r>
-            </a:p>
-          </xdr:txBody>
-        </xdr:sp>
-        <xdr:clientData/>
-      </xdr:twoCellAnchor>
-    </mc:Choice>
-    <mc:Fallback/>
-  </mc:AlternateContent>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:twoCellAnchor editAs="oneCell">
-        <xdr:from>
-          <xdr:col>3</xdr:col>
-          <xdr:colOff>58392</xdr:colOff>
-          <xdr:row>15</xdr:row>
-          <xdr:rowOff>21949</xdr:rowOff>
-        </xdr:from>
-        <xdr:to>
-          <xdr:col>4</xdr:col>
-          <xdr:colOff>239367</xdr:colOff>
+          <xdr:colOff>238125</xdr:colOff>
           <xdr:row>16</xdr:row>
-          <xdr:rowOff>88625</xdr:rowOff>
+          <xdr:rowOff>85725</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -506,15 +438,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>3</xdr:col>
-          <xdr:colOff>55908</xdr:colOff>
+          <xdr:colOff>57150</xdr:colOff>
           <xdr:row>15</xdr:row>
-          <xdr:rowOff>184695</xdr:rowOff>
+          <xdr:rowOff>180975</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>313083</xdr:colOff>
+          <xdr:colOff>314325</xdr:colOff>
           <xdr:row>17</xdr:row>
-          <xdr:rowOff>63354</xdr:rowOff>
+          <xdr:rowOff>66675</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -592,13 +524,13 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>3</xdr:col>
-          <xdr:colOff>63360</xdr:colOff>
+          <xdr:colOff>66675</xdr:colOff>
           <xdr:row>17</xdr:row>
           <xdr:rowOff>38100</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>82410</xdr:colOff>
+          <xdr:colOff>85725</xdr:colOff>
           <xdr:row>18</xdr:row>
           <xdr:rowOff>47625</xdr:rowOff>
         </xdr:to>
@@ -664,6 +596,350 @@
                   <a:cs typeface="Segoe UI"/>
                 </a:rPr>
                 <a:t>Check Box 14</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>3</xdr:col>
+          <xdr:colOff>66675</xdr:colOff>
+          <xdr:row>13</xdr:row>
+          <xdr:rowOff>95250</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>228600</xdr:colOff>
+          <xdr:row>14</xdr:row>
+          <xdr:rowOff>161925</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1039" name="Check Box 15" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1039"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000F040000}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="l" rtl="0">
+                <a:defRPr sz="1000"/>
+              </a:pPr>
+              <a:r>
+                <a:rPr lang="ko-KR" altLang="en-US" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                  <a:solidFill>
+                    <a:srgbClr val="000000"/>
+                  </a:solidFill>
+                  <a:latin typeface="Segoe UI"/>
+                  <a:cs typeface="Segoe UI"/>
+                </a:rPr>
+                <a:t>Check Box 15</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>3</xdr:col>
+          <xdr:colOff>104775</xdr:colOff>
+          <xdr:row>19</xdr:row>
+          <xdr:rowOff>66675</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>371475</xdr:colOff>
+          <xdr:row>20</xdr:row>
+          <xdr:rowOff>76200</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1040" name="Check Box 16" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1040"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000010040000}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="l" rtl="0">
+                <a:defRPr sz="1000"/>
+              </a:pPr>
+              <a:r>
+                <a:rPr lang="ko-KR" altLang="en-US" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                  <a:solidFill>
+                    <a:srgbClr val="000000"/>
+                  </a:solidFill>
+                  <a:latin typeface="Segoe UI"/>
+                  <a:cs typeface="Segoe UI"/>
+                </a:rPr>
+                <a:t>Check Box 16</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>209550</xdr:colOff>
+          <xdr:row>21</xdr:row>
+          <xdr:rowOff>57150</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>266700</xdr:colOff>
+          <xdr:row>22</xdr:row>
+          <xdr:rowOff>66675</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1042" name="Check Box 18" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1042"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000012040000}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="l" rtl="0">
+                <a:defRPr sz="1000"/>
+              </a:pPr>
+              <a:r>
+                <a:rPr lang="ko-KR" altLang="en-US" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                  <a:solidFill>
+                    <a:srgbClr val="000000"/>
+                  </a:solidFill>
+                  <a:latin typeface="Segoe UI"/>
+                  <a:cs typeface="Segoe UI"/>
+                </a:rPr>
+                <a:t>Check Box 18</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>219075</xdr:colOff>
+          <xdr:row>23</xdr:row>
+          <xdr:rowOff>28575</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>390525</xdr:colOff>
+          <xdr:row>24</xdr:row>
+          <xdr:rowOff>38100</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1043" name="Check Box 19" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1043"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000013040000}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="l" rtl="0">
+                <a:defRPr sz="1000"/>
+              </a:pPr>
+              <a:r>
+                <a:rPr lang="ko-KR" altLang="en-US" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                  <a:solidFill>
+                    <a:srgbClr val="000000"/>
+                  </a:solidFill>
+                  <a:latin typeface="Segoe UI"/>
+                  <a:cs typeface="Segoe UI"/>
+                </a:rPr>
+                <a:t>Check Box 19</a:t>
               </a:r>
             </a:p>
           </xdr:txBody>
@@ -976,7 +1252,7 @@
   <dimension ref="C3:G11"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1026,29 +1302,7 @@
       <controls>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1025" r:id="rId4" name="Check Box 1">
-              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
-                <anchor moveWithCells="1">
-                  <from>
-                    <xdr:col>3</xdr:col>
-                    <xdr:colOff>57150</xdr:colOff>
-                    <xdr:row>14</xdr:row>
-                    <xdr:rowOff>95250</xdr:rowOff>
-                  </from>
-                  <to>
-                    <xdr:col>4</xdr:col>
-                    <xdr:colOff>523875</xdr:colOff>
-                    <xdr:row>15</xdr:row>
-                    <xdr:rowOff>104775</xdr:rowOff>
-                  </to>
-                </anchor>
-              </controlPr>
-            </control>
-          </mc:Choice>
-        </mc:AlternateContent>
-        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-          <mc:Choice Requires="x14">
-            <control shapeId="1035" r:id="rId5" name="Check Box 11">
+            <control shapeId="1035" r:id="rId4" name="Check Box 11">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -1070,7 +1324,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1036" r:id="rId6" name="Check Box 12">
+            <control shapeId="1036" r:id="rId5" name="Check Box 12">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -1092,7 +1346,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1038" r:id="rId7" name="Check Box 14">
+            <control shapeId="1038" r:id="rId6" name="Check Box 14">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -1112,6 +1366,94 @@
             </control>
           </mc:Choice>
         </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1039" r:id="rId7" name="Check Box 15">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>3</xdr:col>
+                    <xdr:colOff>66675</xdr:colOff>
+                    <xdr:row>13</xdr:row>
+                    <xdr:rowOff>95250</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>4</xdr:col>
+                    <xdr:colOff>228600</xdr:colOff>
+                    <xdr:row>14</xdr:row>
+                    <xdr:rowOff>161925</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1040" r:id="rId8" name="Check Box 16">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>3</xdr:col>
+                    <xdr:colOff>104775</xdr:colOff>
+                    <xdr:row>19</xdr:row>
+                    <xdr:rowOff>66675</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>4</xdr:col>
+                    <xdr:colOff>371475</xdr:colOff>
+                    <xdr:row>20</xdr:row>
+                    <xdr:rowOff>76200</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1042" r:id="rId9" name="Check Box 18">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>2</xdr:col>
+                    <xdr:colOff>209550</xdr:colOff>
+                    <xdr:row>21</xdr:row>
+                    <xdr:rowOff>57150</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>4</xdr:col>
+                    <xdr:colOff>266700</xdr:colOff>
+                    <xdr:row>22</xdr:row>
+                    <xdr:rowOff>66675</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1043" r:id="rId10" name="Check Box 19">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>2</xdr:col>
+                    <xdr:colOff>219075</xdr:colOff>
+                    <xdr:row>23</xdr:row>
+                    <xdr:rowOff>28575</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>4</xdr:col>
+                    <xdr:colOff>390525</xdr:colOff>
+                    <xdr:row>24</xdr:row>
+                    <xdr:rowOff>38100</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
       </controls>
     </mc:Choice>
   </mc:AlternateContent>

</xml_diff>